<commit_message>
Fixed CMA and ANL instability, converted .json config files to Excel
</commit_message>
<xml_diff>
--- a/data/Hamburg Port Code Mapping.xlsx
+++ b/data/Hamburg Port Code Mapping.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tym.Teo\Documents\Delay Report - Rewrite\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA57E67C-E226-430B-A87B-127E6AC2F20E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15B4D59-2A63-4A2D-A3EA-8E189B12E3A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="OOCL" sheetId="2" r:id="rId1"/>
+    <sheet name="Hamburg" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="7" state="hidden" r:id="rId2"/>
     <sheet name="CMA" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OOCL!$A$1:$B$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hamburg!$A$1:$B$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -651,7 +651,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1177,6 +1177,7 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1666,6 +1667,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003B07C177EC98944892D6859FC7228F27" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fa0312146baf983fe551619124602045">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cadb0006-b086-403f-9c46-c0186d7f6965" xmlns:ns3="4af93f69-0cef-4f40-803d-f637351e1512" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c8aa75208339fe16869b5142f429bf55" ns2:_="" ns3:_="">
     <xsd:import namespace="cadb0006-b086-403f-9c46-c0186d7f6965"/>
@@ -1882,12 +1889,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01DD0693-FE4D-4885-BF24-94BEA9248921}">
   <ds:schemaRefs>
@@ -1897,6 +1898,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE68490-0574-4399-8E76-2FC2ACED3CAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80FBAC62-C129-4627-A795-495E3326B79B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1913,13 +1923,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE68490-0574-4399-8E76-2FC2ACED3CAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>